<commit_message>
13th commit final version
</commit_message>
<xml_diff>
--- a/src/example3.xlsx
+++ b/src/example3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Наименование валюты</t>
   </si>
@@ -20,10 +20,7 @@
     <t>Курс к RUB</t>
   </si>
   <si>
-    <t>египетских фунтов</t>
-  </si>
-  <si>
-    <t>фунт стерлингов соединенного королевства</t>
+    <t>BGN</t>
   </si>
 </sst>
 </file>
@@ -68,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -87,15 +84,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>26.113800048828125</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>99.50350189208984</v>
+        <v>44.204898834228516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
14th commit release version with new interface
</commit_message>
<xml_diff>
--- a/src/example3.xlsx
+++ b/src/example3.xlsx
@@ -20,7 +20,7 @@
     <t>Курс к RUB</t>
   </si>
   <si>
-    <t>BGN</t>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -84,7 +84,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>44.204898834228516</v>
+        <v>80.68720245361328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15th commit release version with new interface amended
</commit_message>
<xml_diff>
--- a/src/example3.xlsx
+++ b/src/example3.xlsx
@@ -12,15 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Наименование валюты</t>
   </si>
   <si>
     <t>Курс к RUB</t>
-  </si>
-  <si>
-    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -65,7 +62,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -79,14 +76,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>80.68720245361328</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
16th final commit working version
</commit_message>
<xml_diff>
--- a/src/example3.xlsx
+++ b/src/example3.xlsx
@@ -12,12 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Наименование валюты</t>
   </si>
   <si>
     <t>Курс к RUB</t>
+  </si>
+  <si>
+    <t>египетских фунтов</t>
+  </si>
+  <si>
+    <t>фунт стерлингов соединенного королевства</t>
   </si>
 </sst>
 </file>
@@ -62,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -76,6 +82,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>26.113800048828125</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>99.50350189208984</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>